<commit_message>
payment order excel file
</commit_message>
<xml_diff>
--- a/payment order.xlsx
+++ b/payment order.xlsx
@@ -120,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -210,17 +210,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -354,11 +343,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -367,22 +353,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -391,16 +364,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -409,17 +374,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,13 +746,14 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:L9"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
     <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" customWidth="1"/>
@@ -769,7 +762,7 @@
     <col min="8" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="4.85546875" customWidth="1"/>
-    <col min="11" max="11" width="3.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" customWidth="1"/>
     <col min="13" max="13" width="5.7109375" customWidth="1"/>
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
@@ -779,395 +772,397 @@
   <sheetData>
     <row r="1" spans="1:22" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="15"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="6" t="s">
+      <c r="A3" s="13"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="16" t="s">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="9"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="9"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="6"/>
       <c r="P4" t="s">
         <v>14</v>
       </c>
       <c r="Q4" t="s">
         <v>7</v>
       </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="16" t="s">
+      <c r="A5" s="13"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="9"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="6"/>
       <c r="P5" t="s">
         <v>15</v>
       </c>
       <c r="Q5" t="s">
         <v>8</v>
       </c>
-      <c r="T5" s="4"/>
-      <c r="U5" s="2"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="1"/>
     </row>
     <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="14"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
       <c r="Q6" t="s">
         <v>9</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="9"/>
+      <c r="A7" s="13"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="6"/>
       <c r="Q7" t="s">
         <v>10</v>
       </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="6"/>
       <c r="Q8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="36" t="s">
+      <c r="A9" s="13"/>
+      <c r="B9" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="2" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="9"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="6"/>
       <c r="Q9" t="s">
         <v>12</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="A10" s="13"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="4" t="s">
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="9"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="D11" s="28"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="9"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="9"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="2"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="9"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="1:22" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="9"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="34" t="s">
+      <c r="A17" s="13"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="33" t="s">
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="34"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="29" t="s">
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="2" t="s">
+      <c r="J17" s="1"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="23"/>
+      <c r="M17" s="13"/>
     </row>
     <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="23"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="36" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="36" t="s">
+      <c r="G19" s="4"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="36" t="s">
+      <c r="J19" s="1"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="23"/>
+      <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="32"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="F6:I6"/>
+  <mergeCells count="11">
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="F3:I4"/>
     <mergeCell ref="D3:D6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="F6:I6"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I10">

</xml_diff>